<commit_message>
Modified the plan and formatted the code.
</commit_message>
<xml_diff>
--- a/docs/dev-plan-draft.xlsx
+++ b/docs/dev-plan-draft.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace-web\mdh\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\busheng.xi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="9300" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Quick Search</t>
   </si>
   <si>
-    <t>Clear all fields</t>
-  </si>
-  <si>
     <t>Loading state of search</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>Textbox design with title and value in same box</t>
   </si>
   <si>
-    <t>Quick search presentation, value being selected on all input boxes</t>
-  </si>
-  <si>
     <t>Time box select options</t>
   </si>
   <si>
@@ -267,35 +261,6 @@
   </si>
   <si>
     <t>This is a reusable UI control, also used in Transaction Details Page</t>
-  </si>
-  <si>
-    <t>The back end should at least be divided into 2 layers. Use a Model/Controller architecture.
-1. At the controller layer, it handles requests sent from the user agent( web browser, mobile browser, or programable HTTP requests ). 
-2. At the model layer, it mainly works with database. And other data,  either static or dynamic, for example, 
-Eg.1 a map between Transaction ID and types, and/or
-Eg.2 a map between Service order types and sub-types
-should also be in model layer.
-Controller layer purpose:
-1. Handles requests of normal data queries, eg. transactions, transaction details, transaction status
-2. Handle users relevant requests, eg. user' profile. 
-3. Handle user's status, eg. login/logout, online, login timeout, etc.
-4. Handle user agent's status, eg. clear browser cookie, browser cache, browser being closed, etc.
-5. Handle user input errors, invalid user input, unsafe data, malicious data, etc.
-6. Handle server errors, 404, 500, etc.
-Controller architecture - multiple layers
-Layer 1: Validate and sanitise requests
-Layer 2: Detect user agents, make redirections, handle cookies, etc
-Layer 3: Add global response headers
-Layer 4: Handle each mapping requests
-Layer 5: Add analytical and/or statistical code( if applicable )
-Model Layer purpose:
-0. Do not use ORM. Ideally, each request from Controller layer should be completed by only one SQL query or one database transaction.
-1. Every request must only get/update the data of database from model layer( model module ).
-2. Manage database connections, eg. connection pool
-3. Manage data cache.
-4. Obtain data from database and make it into desired format
-5. Use data from controller layer to update the database.
-Model Layer architecture - TBD</t>
   </si>
   <si>
     <t>Dropdown scrollbar( third party UI controller )</t>
@@ -332,6 +297,39 @@
   </si>
   <si>
     <t>UI test of Details page may start</t>
+  </si>
+  <si>
+    <t>The back end should at least be divided into 2 layers. Use a Model/Controller architecture.
+1. At the controller layer, it handles requests sent from the user agent( web browser, mobile browser, or programable HTTP requests ). 
+2. At the model layer, it mainly works with database. And other data,  either static or dynamic, for example, 
+Eg.1 a map between Transaction ID and types, and/or
+Eg.2 a map between Service order types and sub-types
+should also be in model layer.
+Controller layer purpose:
+1. Handles requests of normal data queries, eg. transactions, transaction details, transaction status
+2. Handle users relevant requests, eg. user' profile. 
+3. Handle user's status, eg. login/logout, online, login timeout, etc.
+4. Handle user agent's status, eg. clear browser cookie, browser cache, browser being closed, etc.
+5. Handle user input errors, invalid user input, unsafe data, malicious data, etc.
+6. Handle server errors, 404, 500, etc.
+Controller architecture - multiple layers - life cycle.
+Layer 1: Authentication and authorisation
+Layer 2: Validate and sanitise requests
+Layer 3: Detect headers, decide if data should be pulled from database or use browsers's local data, make redirections, handle cookies, etc
+Layer 4: Request data from model layer - Model layer should decdide to use a cached version or perform queries to database
+Layer 5: Add global response headers
+Layer 6: Add analytical and/or statistical code( if applicable )
+Model Layer purpose:
+0. Do not use ORM. Ideally, each request from Controller layer should be completed by only one SQL query or one database transaction.
+1. Every request must only get/update the data of database from model layer( model module ).
+2. Manage database connections, eg. connection pool
+3. Manage data cache.
+4. Obtain data from database and make it into desired format
+5. Use data from controller layer to update the database.
+Model Layer architecture - TBD</t>
+  </si>
+  <si>
+    <t>Clear all fields - from UI, data layer, local storage</t>
   </si>
 </sst>
 </file>
@@ -462,40 +460,40 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -826,25 +824,25 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="28" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" style="22" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="15.85546875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -852,19 +850,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>76</v>
+      <c r="F1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -876,15 +874,15 @@
         <v>Tuesday</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>82</v>
+      <c r="F2" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -899,11 +897,11 @@
         <v>7</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
+      <c r="E3" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -917,9 +915,9 @@
         <v>5</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -933,9 +931,9 @@
         <v>5</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -945,9 +943,9 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -958,9 +956,9 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -975,9 +973,9 @@
         <v>3</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -991,9 +989,9 @@
         <v>3</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -1007,9 +1005,9 @@
         <v>3</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1023,9 +1021,9 @@
         <v>4</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1039,9 +1037,9 @@
         <v>4</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1054,8 +1052,8 @@
       <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1067,8 +1065,8 @@
         <v>Sunday</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1084,8 +1082,8 @@
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1100,10 +1098,10 @@
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>42914</v>
       </c>
@@ -1112,12 +1110,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1128,12 +1126,12 @@
         <v>Thursday</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -1144,12 +1142,12 @@
         <v>Friday</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1160,10 +1158,10 @@
         <v>Saturday</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+        <v>10</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1174,8 +1172,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1187,12 +1185,12 @@
         <v>Monday</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -1203,12 +1201,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1219,12 +1217,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -1235,12 +1233,12 @@
         <v>Thursday</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1251,12 +1249,12 @@
         <v>Friday</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -1266,8 +1264,8 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1278,8 +1276,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1291,12 +1289,12 @@
         <v>Monday</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1307,12 +1305,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -1323,12 +1321,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -1339,14 +1337,14 @@
         <v>Thursday</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
-    </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>42930</v>
       </c>
@@ -1355,12 +1353,12 @@
         <v>Friday</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -1370,8 +1368,8 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1382,8 +1380,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1395,12 +1393,12 @@
         <v>Monday</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
@@ -1411,12 +1409,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="26"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -1427,12 +1425,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="26"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -1443,12 +1441,12 @@
         <v>Thursday</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
@@ -1459,12 +1457,12 @@
         <v>Friday</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="26"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -1474,8 +1472,8 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="29"/>
       <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1486,8 +1484,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
       <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1499,12 +1497,12 @@
         <v>Monday</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1515,12 +1513,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="26"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
@@ -1531,12 +1529,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="26"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
@@ -1547,14 +1545,14 @@
         <v>Thursday</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="26"/>
-    </row>
-    <row r="47" spans="1:8" s="23" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+    </row>
+    <row r="47" spans="1:8" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>42944</v>
       </c>
@@ -1563,14 +1561,14 @@
         <v>Friday</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
+        <v>32</v>
+      </c>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -1581,8 +1579,8 @@
         <v>Saturday</v>
       </c>
       <c r="C48" s="4"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="29"/>
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1594,8 +1592,8 @@
         <v>Sunday</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="29"/>
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1607,14 +1605,14 @@
         <v>Monday</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E50" s="7"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="26"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
@@ -1625,14 +1623,14 @@
         <v>Tuesday</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="26"/>
-    </row>
-    <row r="52" spans="1:8" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+    </row>
+    <row r="52" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>42949</v>
       </c>
@@ -1641,14 +1639,14 @@
         <v>Wednesday</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F52" s="25"/>
-      <c r="G52" s="26"/>
+        <v>33</v>
+      </c>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1659,14 +1657,14 @@
         <v>Thursday</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E53" s="7"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="26"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
     </row>
     <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1677,12 +1675,12 @@
         <v>Friday</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="26"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -1693,8 +1691,8 @@
         <v>Saturday</v>
       </c>
       <c r="C55" s="4"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="29"/>
     </row>
     <row r="56" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
@@ -1705,8 +1703,8 @@
         <v>Sunday</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="29"/>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1717,12 +1715,12 @@
         <v>Monday</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="26"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
@@ -1733,12 +1731,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="26"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1749,12 +1747,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="26"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
     </row>
     <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
@@ -1765,12 +1763,12 @@
         <v>Thursday</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="26"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
@@ -1781,12 +1779,12 @@
         <v>Friday</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="26"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
     </row>
     <row r="62" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
@@ -1797,8 +1795,8 @@
         <v>Saturday</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="29"/>
     </row>
     <row r="63" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
@@ -1809,8 +1807,8 @@
         <v>Sunday</v>
       </c>
       <c r="C63" s="4"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="29"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -1821,12 +1819,12 @@
         <v>Monday</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="26"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="27"/>
     </row>
     <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
@@ -1837,12 +1835,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="26"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
@@ -1853,12 +1851,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="26"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27"/>
     </row>
     <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
@@ -1869,14 +1867,14 @@
         <v>Thursday</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F67" s="25"/>
-      <c r="G67" s="26"/>
+        <v>49</v>
+      </c>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
@@ -1887,12 +1885,12 @@
         <v>Friday</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="26"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
     </row>
     <row r="69" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -1902,8 +1900,8 @@
         <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="29"/>
     </row>
     <row r="70" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
@@ -1913,8 +1911,8 @@
         <f t="shared" si="1"/>
         <v>Sunday</v>
       </c>
-      <c r="F70" s="19"/>
-      <c r="G70" s="19"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="29"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
@@ -1925,12 +1923,12 @@
         <v>Monday</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="26"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="27"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
@@ -1941,12 +1939,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="26"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
@@ -1957,12 +1955,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="26"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="27"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
@@ -1973,12 +1971,12 @@
         <v>Thursday</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="26"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="27"/>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
@@ -1989,12 +1987,12 @@
         <v>Friday</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="26"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
@@ -2005,8 +2003,8 @@
         <v>Saturday</v>
       </c>
       <c r="C76" s="4"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="29"/>
     </row>
     <row r="77" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
@@ -2017,8 +2015,8 @@
         <v>Sunday</v>
       </c>
       <c r="C77" s="4"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="29"/>
     </row>
     <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
@@ -2029,12 +2027,12 @@
         <v>Monday</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="26"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="27"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
@@ -2045,12 +2043,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="26"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="27"/>
     </row>
     <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
@@ -2061,14 +2059,14 @@
         <v>Wednesday</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F80" s="25"/>
-      <c r="G80" s="26"/>
+        <v>52</v>
+      </c>
+      <c r="F80" s="27"/>
+      <c r="G80" s="27"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
@@ -2079,14 +2077,14 @@
         <v>Thursday</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="26"/>
-    </row>
-    <row r="82" spans="1:7" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+    </row>
+    <row r="82" spans="1:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>42979</v>
       </c>
@@ -2095,14 +2093,14 @@
         <v>Friday</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D82" s="11"/>
       <c r="E82" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F82" s="25"/>
-      <c r="G82" s="26"/>
+        <v>57</v>
+      </c>
+      <c r="F82" s="27"/>
+      <c r="G82" s="27"/>
     </row>
     <row r="83" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
@@ -2113,8 +2111,8 @@
         <v>Saturday</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="29"/>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
@@ -2125,10 +2123,10 @@
         <v>Sunday</v>
       </c>
       <c r="C84" s="4"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="19"/>
-    </row>
-    <row r="85" spans="1:7" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F84" s="28"/>
+      <c r="G84" s="29"/>
+    </row>
+    <row r="85" spans="1:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>42982</v>
       </c>
@@ -2137,12 +2135,12 @@
         <v>Monday</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
-      <c r="F85" s="25"/>
-      <c r="G85" s="26"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="27"/>
     </row>
     <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
@@ -2153,14 +2151,14 @@
         <v>Tuesday</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E86" s="7"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="26"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="27"/>
     </row>
     <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
@@ -2171,12 +2169,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="26"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
@@ -2187,12 +2185,12 @@
         <v>Thursday</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="26"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="27"/>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
@@ -2203,12 +2201,12 @@
         <v>Friday</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="26"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
     </row>
     <row r="90" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
@@ -2219,8 +2217,8 @@
         <v>Saturday</v>
       </c>
       <c r="C90" s="4"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="19"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="29"/>
     </row>
     <row r="91" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
@@ -2231,8 +2229,8 @@
         <v>Sunday</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="19"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="29"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
@@ -2243,12 +2241,12 @@
         <v>Monday</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="26"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="27"/>
     </row>
     <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
@@ -2259,12 +2257,12 @@
         <v>Tuesday</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="26"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="27"/>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
@@ -2275,12 +2273,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="26"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="27"/>
     </row>
     <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
@@ -2291,14 +2289,14 @@
         <v>Thursday</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="26"/>
-    </row>
-    <row r="96" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F95" s="27"/>
+      <c r="G95" s="27"/>
+    </row>
+    <row r="96" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>42993</v>
       </c>
@@ -2307,14 +2305,14 @@
         <v>Friday</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F96" s="25"/>
-      <c r="G96" s="26"/>
+        <v>50</v>
+      </c>
+      <c r="F96" s="27"/>
+      <c r="G96" s="27"/>
     </row>
     <row r="97" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
@@ -2325,8 +2323,8 @@
         <v>Saturday</v>
       </c>
       <c r="C97" s="4"/>
-      <c r="F97" s="19"/>
-      <c r="G97" s="19"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="29"/>
     </row>
     <row r="98" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
@@ -2337,8 +2335,8 @@
         <v>Sunday</v>
       </c>
       <c r="C98" s="4"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="19"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="29"/>
     </row>
     <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
@@ -2349,16 +2347,16 @@
         <v>Monday</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E99" s="7"/>
-      <c r="F99" s="25"/>
-      <c r="G99" s="26"/>
-    </row>
-    <row r="100" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F99" s="27"/>
+      <c r="G99" s="27"/>
+    </row>
+    <row r="100" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <v>42997</v>
       </c>
@@ -2367,16 +2365,16 @@
         <v>Tuesday</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D100" s="17"/>
       <c r="E100" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F100" s="25"/>
-      <c r="G100" s="26"/>
-    </row>
-    <row r="101" spans="1:7" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+    </row>
+    <row r="101" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <v>42998</v>
       </c>
@@ -2385,12 +2383,12 @@
         <v>Wednesday</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D101" s="17"/>
       <c r="E101" s="17"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="26"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
@@ -2402,11 +2400,11 @@
       </c>
       <c r="C102" s="7"/>
       <c r="D102" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E102" s="7"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="26"/>
+      <c r="F102" s="27"/>
+      <c r="G102" s="27"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
@@ -2419,8 +2417,8 @@
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="26"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="27"/>
     </row>
     <row r="104" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
@@ -2431,8 +2429,8 @@
         <v>Saturday</v>
       </c>
       <c r="C104" s="4"/>
-      <c r="F104" s="19"/>
-      <c r="G104" s="19"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="29"/>
     </row>
     <row r="105" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
@@ -2443,8 +2441,8 @@
         <v>Sunday</v>
       </c>
       <c r="C105" s="4"/>
-      <c r="F105" s="19"/>
-      <c r="G105" s="19"/>
+      <c r="F105" s="28"/>
+      <c r="G105" s="29"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
@@ -2457,8 +2455,8 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="26"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="27"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
@@ -2471,8 +2469,8 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
-      <c r="F107" s="25"/>
-      <c r="G107" s="26"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
@@ -2485,8 +2483,8 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
-      <c r="F108" s="25"/>
-      <c r="G108" s="26"/>
+      <c r="F108" s="27"/>
+      <c r="G108" s="27"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
@@ -2499,8 +2497,8 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="26"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
@@ -2513,8 +2511,8 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
-      <c r="F110" s="25"/>
-      <c r="G110" s="26"/>
+      <c r="F110" s="27"/>
+      <c r="G110" s="27"/>
     </row>
     <row r="111" spans="1:7" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">

</xml_diff>

<commit_message>
Modified DropdownBox logic and added disable feature of DropdownBox.
</commit_message>
<xml_diff>
--- a/docs/dev-plan-draft.xlsx
+++ b/docs/dev-plan-draft.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\busheng.xi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace-web\mdh\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -331,6 +331,9 @@
   <si>
     <t>Clear all fields - from UI, data layer, local storage</t>
   </si>
+  <si>
+    <t>State ( Green is done, yellow is not required )</t>
+  </si>
 </sst>
 </file>
 
@@ -356,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +381,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -494,6 +509,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -822,11 +843,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,15 +855,16 @@
     <col min="1" max="1" width="15.85546875" style="23" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="24" customWidth="1"/>
     <col min="3" max="3" width="39.42578125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" style="19" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="19"/>
+    <col min="4" max="4" width="5.5703125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="38.42578125" style="19" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="19" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -853,19 +875,22 @@
         <v>75</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>42899</v>
       </c>
@@ -876,16 +901,17 @@
       <c r="C2" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="H2" s="27" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>42900</v>
       </c>
@@ -897,13 +923,14 @@
         <v>7</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="27"/>
       <c r="G3" s="27"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>42901</v>
       </c>
@@ -914,12 +941,13 @@
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="27"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="27"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="27"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>42902</v>
       </c>
@@ -930,12 +958,13 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="27"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42903</v>
       </c>
@@ -943,12 +972,12 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="26"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42904</v>
       </c>
@@ -956,12 +985,12 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="26"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>42905</v>
       </c>
@@ -972,12 +1001,13 @@
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="27"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>42906</v>
       </c>
@@ -988,12 +1018,13 @@
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="27"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>42907</v>
       </c>
@@ -1004,12 +1035,13 @@
       <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="27"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>42908</v>
       </c>
@@ -1020,12 +1052,13 @@
       <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="27"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="27"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>42909</v>
       </c>
@@ -1036,12 +1069,13 @@
       <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="27"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="27"/>
-    </row>
-    <row r="13" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42910</v>
       </c>
@@ -1052,11 +1086,12 @@
       <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="4"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42911</v>
       </c>
@@ -1065,11 +1100,12 @@
         <v>Sunday</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="4"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>42912</v>
       </c>
@@ -1080,12 +1116,13 @@
       <c r="C15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="27"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>42913</v>
       </c>
@@ -1096,12 +1133,13 @@
       <c r="C16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="27"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>42914</v>
       </c>
@@ -1114,10 +1152,11 @@
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="27"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="27"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="27"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>42915</v>
       </c>
@@ -1130,10 +1169,11 @@
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="27"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="27"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>42916</v>
       </c>
@@ -1146,10 +1186,11 @@
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="27"/>
+    </row>
+    <row r="20" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42917</v>
       </c>
@@ -1160,11 +1201,12 @@
       <c r="C20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="4"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42918</v>
       </c>
@@ -1172,11 +1214,11 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>42919</v>
       </c>
@@ -1189,10 +1231,11 @@
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="27"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>42920</v>
       </c>
@@ -1205,10 +1248,11 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="27"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>42921</v>
       </c>
@@ -1221,10 +1265,11 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="27"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>42922</v>
       </c>
@@ -1235,12 +1280,13 @@
       <c r="C25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="27"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="27"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>42923</v>
       </c>
@@ -1251,12 +1297,13 @@
       <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="27"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="27"/>
-    </row>
-    <row r="27" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>42924</v>
       </c>
@@ -1264,11 +1311,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="28"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>42925</v>
       </c>
@@ -1276,11 +1323,11 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="28"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>42926</v>
       </c>
@@ -1291,12 +1338,13 @@
       <c r="C29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="27"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="27"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="27"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>42927</v>
       </c>
@@ -1309,10 +1357,11 @@
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="27"/>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H30" s="27"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>42928</v>
       </c>
@@ -1325,10 +1374,11 @@
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="27"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="27"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>42929</v>
       </c>
@@ -1341,10 +1391,11 @@
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="27"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="27"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>42930</v>
       </c>
@@ -1357,10 +1408,11 @@
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="27"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="27"/>
-    </row>
-    <row r="34" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="27"/>
+    </row>
+    <row r="34" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>42931</v>
       </c>
@@ -1368,11 +1420,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="8"/>
-    </row>
-    <row r="35" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="28"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>42932</v>
       </c>
@@ -1380,11 +1432,11 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="28"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>42933</v>
       </c>
@@ -1397,10 +1449,11 @@
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="27"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="27"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="27"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>42934</v>
       </c>
@@ -1413,10 +1466,11 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="27"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="27"/>
-    </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H37" s="27"/>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>42935</v>
       </c>
@@ -1427,12 +1481,13 @@
       <c r="C38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="7"/>
+      <c r="D38" s="31"/>
       <c r="E38" s="7"/>
-      <c r="F38" s="27"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="27"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>42936</v>
       </c>
@@ -1445,10 +1500,11 @@
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
-      <c r="F39" s="27"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="27"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="27"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>42937</v>
       </c>
@@ -1461,10 +1517,11 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="27"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="27"/>
+    </row>
+    <row r="41" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>42938</v>
       </c>
@@ -1472,11 +1529,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="F41" s="28"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="28"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>42939</v>
       </c>
@@ -1484,11 +1541,11 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F42" s="28"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="8"/>
-    </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G42" s="28"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42940</v>
       </c>
@@ -1501,10 +1558,11 @@
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="27"/>
+      <c r="F43" s="7"/>
       <c r="G43" s="27"/>
-    </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H43" s="27"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>42941</v>
       </c>
@@ -1517,10 +1575,11 @@
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="27"/>
+      <c r="F44" s="7"/>
       <c r="G44" s="27"/>
-    </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H44" s="27"/>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>42942</v>
       </c>
@@ -1533,10 +1592,11 @@
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="27"/>
+      <c r="F45" s="7"/>
       <c r="G45" s="27"/>
-    </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H45" s="27"/>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>42943</v>
       </c>
@@ -1549,10 +1609,11 @@
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="27"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="27"/>
-    </row>
-    <row r="47" spans="1:8" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="H46" s="27"/>
+    </row>
+    <row r="47" spans="1:9" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>42944</v>
       </c>
@@ -1564,13 +1625,14 @@
         <v>30</v>
       </c>
       <c r="D47" s="11"/>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="11"/>
+      <c r="F47" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F47" s="27"/>
       <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="27"/>
+    </row>
+    <row r="48" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>42945</v>
       </c>
@@ -1579,11 +1641,12 @@
         <v>Saturday</v>
       </c>
       <c r="C48" s="4"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="8"/>
-    </row>
-    <row r="49" spans="1:8" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="4"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>42946</v>
       </c>
@@ -1592,11 +1655,12 @@
         <v>Sunday</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="8"/>
-    </row>
-    <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D49" s="4"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>42947</v>
       </c>
@@ -1607,14 +1671,15 @@
       <c r="C50" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="7"/>
+      <c r="E50" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E50" s="7"/>
-      <c r="F50" s="27"/>
+      <c r="F50" s="7"/>
       <c r="G50" s="27"/>
-    </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H50" s="27"/>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>42948</v>
       </c>
@@ -1627,10 +1692,11 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
-      <c r="F51" s="27"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="27"/>
-    </row>
-    <row r="52" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H51" s="27"/>
+    </row>
+    <row r="52" spans="1:9" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>42949</v>
       </c>
@@ -1642,13 +1708,14 @@
         <v>31</v>
       </c>
       <c r="D52" s="11"/>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="11"/>
+      <c r="F52" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F52" s="27"/>
       <c r="G52" s="27"/>
-    </row>
-    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H52" s="27"/>
+    </row>
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>42950</v>
       </c>
@@ -1659,14 +1726,15 @@
       <c r="C53" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="31"/>
+      <c r="E53" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="F53" s="27"/>
+      <c r="F53" s="7"/>
       <c r="G53" s="27"/>
-    </row>
-    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H53" s="27"/>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>42951</v>
       </c>
@@ -1677,12 +1745,13 @@
       <c r="C54" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="7"/>
+      <c r="D54" s="31"/>
       <c r="E54" s="7"/>
-      <c r="F54" s="27"/>
+      <c r="F54" s="7"/>
       <c r="G54" s="27"/>
-    </row>
-    <row r="55" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="27"/>
+    </row>
+    <row r="55" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>42952</v>
       </c>
@@ -1691,10 +1760,11 @@
         <v>Saturday</v>
       </c>
       <c r="C55" s="4"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="29"/>
-    </row>
-    <row r="56" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="4"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="29"/>
+    </row>
+    <row r="56" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>42953</v>
       </c>
@@ -1703,10 +1773,11 @@
         <v>Sunday</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="29"/>
-    </row>
-    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D56" s="4"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="29"/>
+    </row>
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>42954</v>
       </c>
@@ -1717,12 +1788,13 @@
       <c r="C57" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D57" s="7"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="7"/>
-      <c r="F57" s="27"/>
+      <c r="F57" s="7"/>
       <c r="G57" s="27"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H57" s="27"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>42955</v>
       </c>
@@ -1733,12 +1805,13 @@
       <c r="C58" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="7"/>
+      <c r="D58" s="31"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="27"/>
+      <c r="F58" s="7"/>
       <c r="G58" s="27"/>
-    </row>
-    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H58" s="27"/>
+    </row>
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>42956</v>
       </c>
@@ -1749,12 +1822,13 @@
       <c r="C59" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="7"/>
+      <c r="D59" s="31"/>
       <c r="E59" s="7"/>
-      <c r="F59" s="27"/>
+      <c r="F59" s="7"/>
       <c r="G59" s="27"/>
-    </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H59" s="27"/>
+    </row>
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>42957</v>
       </c>
@@ -1765,12 +1839,13 @@
       <c r="C60" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D60" s="7"/>
+      <c r="D60" s="31"/>
       <c r="E60" s="7"/>
-      <c r="F60" s="27"/>
+      <c r="F60" s="7"/>
       <c r="G60" s="27"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="27"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>42958</v>
       </c>
@@ -1781,12 +1856,13 @@
       <c r="C61" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="7"/>
+      <c r="D61" s="31"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="27"/>
+      <c r="F61" s="7"/>
       <c r="G61" s="27"/>
-    </row>
-    <row r="62" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="27"/>
+    </row>
+    <row r="62" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>42959</v>
       </c>
@@ -1795,10 +1871,11 @@
         <v>Saturday</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="29"/>
-    </row>
-    <row r="63" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="4"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="29"/>
+    </row>
+    <row r="63" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>42960</v>
       </c>
@@ -1807,10 +1884,11 @@
         <v>Sunday</v>
       </c>
       <c r="C63" s="4"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="29"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D63" s="4"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="29"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>42961</v>
       </c>
@@ -1821,12 +1899,13 @@
       <c r="C64" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D64" s="7"/>
+      <c r="D64" s="31"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="27"/>
+      <c r="F64" s="7"/>
       <c r="G64" s="27"/>
-    </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H64" s="27"/>
+    </row>
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>42962</v>
       </c>
@@ -1837,12 +1916,13 @@
       <c r="C65" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="7"/>
+      <c r="D65" s="31"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="27"/>
+      <c r="F65" s="7"/>
       <c r="G65" s="27"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="27"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>42963</v>
       </c>
@@ -1853,12 +1933,13 @@
       <c r="C66" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D66" s="7"/>
+      <c r="D66" s="31"/>
       <c r="E66" s="7"/>
-      <c r="F66" s="27"/>
+      <c r="F66" s="7"/>
       <c r="G66" s="27"/>
-    </row>
-    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H66" s="27"/>
+    </row>
+    <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>42964</v>
       </c>
@@ -1869,14 +1950,15 @@
       <c r="C67" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7" t="s">
+      <c r="D67" s="31"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F67" s="27"/>
       <c r="G67" s="27"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="27"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>42965</v>
       </c>
@@ -1887,12 +1969,13 @@
       <c r="C68" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="7"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="7"/>
-      <c r="F68" s="27"/>
+      <c r="F68" s="7"/>
       <c r="G68" s="27"/>
-    </row>
-    <row r="69" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="27"/>
+    </row>
+    <row r="69" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>42966</v>
       </c>
@@ -1900,10 +1983,10 @@
         <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="29"/>
-    </row>
-    <row r="70" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G69" s="28"/>
+      <c r="H69" s="29"/>
+    </row>
+    <row r="70" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>42967</v>
       </c>
@@ -1911,10 +1994,10 @@
         <f t="shared" si="1"/>
         <v>Sunday</v>
       </c>
-      <c r="F70" s="28"/>
-      <c r="G70" s="29"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="28"/>
+      <c r="H70" s="29"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>42968</v>
       </c>
@@ -1925,12 +2008,13 @@
       <c r="C71" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D71" s="7"/>
+      <c r="D71" s="31"/>
       <c r="E71" s="7"/>
-      <c r="F71" s="27"/>
+      <c r="F71" s="7"/>
       <c r="G71" s="27"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="27"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>42969</v>
       </c>
@@ -1941,12 +2025,13 @@
       <c r="C72" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D72" s="7"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="7"/>
-      <c r="F72" s="27"/>
+      <c r="F72" s="7"/>
       <c r="G72" s="27"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="27"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>42970</v>
       </c>
@@ -1957,12 +2042,13 @@
       <c r="C73" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D73" s="7"/>
+      <c r="D73" s="31"/>
       <c r="E73" s="7"/>
-      <c r="F73" s="27"/>
+      <c r="F73" s="7"/>
       <c r="G73" s="27"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="27"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>42971</v>
       </c>
@@ -1973,12 +2059,13 @@
       <c r="C74" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D74" s="7"/>
+      <c r="D74" s="31"/>
       <c r="E74" s="7"/>
-      <c r="F74" s="27"/>
+      <c r="F74" s="7"/>
       <c r="G74" s="27"/>
-    </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H74" s="27"/>
+    </row>
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>42972</v>
       </c>
@@ -1989,12 +2076,13 @@
       <c r="C75" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D75" s="7"/>
+      <c r="D75" s="31"/>
       <c r="E75" s="7"/>
-      <c r="F75" s="27"/>
+      <c r="F75" s="7"/>
       <c r="G75" s="27"/>
-    </row>
-    <row r="76" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="27"/>
+    </row>
+    <row r="76" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>42973</v>
       </c>
@@ -2003,10 +2091,11 @@
         <v>Saturday</v>
       </c>
       <c r="C76" s="4"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="29"/>
-    </row>
-    <row r="77" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D76" s="4"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="29"/>
+    </row>
+    <row r="77" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>42974</v>
       </c>
@@ -2015,10 +2104,11 @@
         <v>Sunday</v>
       </c>
       <c r="C77" s="4"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="29"/>
-    </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D77" s="4"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="29"/>
+    </row>
+    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>42975</v>
       </c>
@@ -2029,12 +2119,13 @@
       <c r="C78" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D78" s="7"/>
+      <c r="D78" s="31"/>
       <c r="E78" s="7"/>
-      <c r="F78" s="27"/>
+      <c r="F78" s="7"/>
       <c r="G78" s="27"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="27"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>42976</v>
       </c>
@@ -2045,12 +2136,13 @@
       <c r="C79" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D79" s="7"/>
+      <c r="D79" s="31"/>
       <c r="E79" s="7"/>
-      <c r="F79" s="27"/>
+      <c r="F79" s="7"/>
       <c r="G79" s="27"/>
-    </row>
-    <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H79" s="27"/>
+    </row>
+    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>42977</v>
       </c>
@@ -2061,14 +2153,15 @@
       <c r="C80" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7" t="s">
+      <c r="D80" s="31"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F80" s="27"/>
       <c r="G80" s="27"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="27"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>42978</v>
       </c>
@@ -2079,12 +2172,13 @@
       <c r="C81" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D81" s="7"/>
+      <c r="D81" s="31"/>
       <c r="E81" s="7"/>
-      <c r="F81" s="27"/>
+      <c r="F81" s="7"/>
       <c r="G81" s="27"/>
-    </row>
-    <row r="82" spans="1:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H81" s="27"/>
+    </row>
+    <row r="82" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>42979</v>
       </c>
@@ -2095,14 +2189,15 @@
       <c r="C82" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11" t="s">
+      <c r="D82" s="31"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F82" s="27"/>
       <c r="G82" s="27"/>
-    </row>
-    <row r="83" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H82" s="27"/>
+    </row>
+    <row r="83" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>42980</v>
       </c>
@@ -2111,10 +2206,11 @@
         <v>Saturday</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="29"/>
-    </row>
-    <row r="84" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="4"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="29"/>
+    </row>
+    <row r="84" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>42981</v>
       </c>
@@ -2123,10 +2219,11 @@
         <v>Sunday</v>
       </c>
       <c r="C84" s="4"/>
-      <c r="F84" s="28"/>
-      <c r="G84" s="29"/>
-    </row>
-    <row r="85" spans="1:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D84" s="4"/>
+      <c r="G84" s="28"/>
+      <c r="H84" s="29"/>
+    </row>
+    <row r="85" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>42982</v>
       </c>
@@ -2137,12 +2234,13 @@
       <c r="C85" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D85" s="11"/>
+      <c r="D85" s="31"/>
       <c r="E85" s="11"/>
-      <c r="F85" s="27"/>
+      <c r="F85" s="11"/>
       <c r="G85" s="27"/>
-    </row>
-    <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H85" s="27"/>
+    </row>
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>42983</v>
       </c>
@@ -2153,14 +2251,15 @@
       <c r="C86" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="7"/>
+      <c r="E86" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E86" s="7"/>
-      <c r="F86" s="27"/>
+      <c r="F86" s="7"/>
       <c r="G86" s="27"/>
-    </row>
-    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H86" s="27"/>
+    </row>
+    <row r="87" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>42984</v>
       </c>
@@ -2173,10 +2272,11 @@
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
-      <c r="F87" s="27"/>
+      <c r="F87" s="7"/>
       <c r="G87" s="27"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="27"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>42985</v>
       </c>
@@ -2189,10 +2289,11 @@
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
-      <c r="F88" s="27"/>
+      <c r="F88" s="7"/>
       <c r="G88" s="27"/>
-    </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H88" s="27"/>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>42986</v>
       </c>
@@ -2205,10 +2306,11 @@
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
-      <c r="F89" s="27"/>
+      <c r="F89" s="7"/>
       <c r="G89" s="27"/>
-    </row>
-    <row r="90" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H89" s="27"/>
+    </row>
+    <row r="90" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>42987</v>
       </c>
@@ -2217,10 +2319,11 @@
         <v>Saturday</v>
       </c>
       <c r="C90" s="4"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="29"/>
-    </row>
-    <row r="91" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D90" s="4"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="29"/>
+    </row>
+    <row r="91" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>42988</v>
       </c>
@@ -2229,10 +2332,11 @@
         <v>Sunday</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="29"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D91" s="4"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="29"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>42989</v>
       </c>
@@ -2245,10 +2349,11 @@
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
-      <c r="F92" s="27"/>
+      <c r="F92" s="7"/>
       <c r="G92" s="27"/>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H92" s="27"/>
+    </row>
+    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>42990</v>
       </c>
@@ -2261,10 +2366,11 @@
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
-      <c r="F93" s="27"/>
+      <c r="F93" s="7"/>
       <c r="G93" s="27"/>
-    </row>
-    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H93" s="27"/>
+    </row>
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>42991</v>
       </c>
@@ -2277,10 +2383,11 @@
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
-      <c r="F94" s="27"/>
+      <c r="F94" s="7"/>
       <c r="G94" s="27"/>
-    </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H94" s="27"/>
+    </row>
+    <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>42992</v>
       </c>
@@ -2293,10 +2400,11 @@
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
-      <c r="F95" s="27"/>
+      <c r="F95" s="7"/>
       <c r="G95" s="27"/>
-    </row>
-    <row r="96" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H95" s="27"/>
+    </row>
+    <row r="96" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>42993</v>
       </c>
@@ -2308,13 +2416,14 @@
         <v>65</v>
       </c>
       <c r="D96" s="11"/>
-      <c r="E96" s="11" t="s">
+      <c r="E96" s="11"/>
+      <c r="F96" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F96" s="27"/>
       <c r="G96" s="27"/>
-    </row>
-    <row r="97" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H96" s="27"/>
+    </row>
+    <row r="97" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>42994</v>
       </c>
@@ -2323,10 +2432,11 @@
         <v>Saturday</v>
       </c>
       <c r="C97" s="4"/>
-      <c r="F97" s="28"/>
-      <c r="G97" s="29"/>
-    </row>
-    <row r="98" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="4"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="29"/>
+    </row>
+    <row r="98" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>42995</v>
       </c>
@@ -2335,10 +2445,11 @@
         <v>Sunday</v>
       </c>
       <c r="C98" s="4"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="29"/>
-    </row>
-    <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D98" s="4"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="29"/>
+    </row>
+    <row r="99" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>42996</v>
       </c>
@@ -2349,14 +2460,15 @@
       <c r="C99" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D99" s="7"/>
+      <c r="E99" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E99" s="7"/>
-      <c r="F99" s="27"/>
+      <c r="F99" s="7"/>
       <c r="G99" s="27"/>
-    </row>
-    <row r="100" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H99" s="27"/>
+    </row>
+    <row r="100" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <v>42997</v>
       </c>
@@ -2368,13 +2480,14 @@
         <v>68</v>
       </c>
       <c r="D100" s="17"/>
-      <c r="E100" s="17" t="s">
+      <c r="E100" s="17"/>
+      <c r="F100" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="F100" s="27"/>
       <c r="G100" s="27"/>
-    </row>
-    <row r="101" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H100" s="27"/>
+    </row>
+    <row r="101" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <v>42998</v>
       </c>
@@ -2387,10 +2500,11 @@
       </c>
       <c r="D101" s="17"/>
       <c r="E101" s="17"/>
-      <c r="F101" s="27"/>
+      <c r="F101" s="17"/>
       <c r="G101" s="27"/>
-    </row>
-    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H101" s="27"/>
+    </row>
+    <row r="102" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>42999</v>
       </c>
@@ -2399,14 +2513,15 @@
         <v>Thursday</v>
       </c>
       <c r="C102" s="7"/>
-      <c r="D102" s="7" t="s">
+      <c r="D102" s="7"/>
+      <c r="E102" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E102" s="7"/>
-      <c r="F102" s="27"/>
+      <c r="F102" s="7"/>
       <c r="G102" s="27"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="27"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>43000</v>
       </c>
@@ -2417,10 +2532,11 @@
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
-      <c r="F103" s="27"/>
+      <c r="F103" s="7"/>
       <c r="G103" s="27"/>
-    </row>
-    <row r="104" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H103" s="27"/>
+    </row>
+    <row r="104" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>43001</v>
       </c>
@@ -2429,10 +2545,11 @@
         <v>Saturday</v>
       </c>
       <c r="C104" s="4"/>
-      <c r="F104" s="28"/>
-      <c r="G104" s="29"/>
-    </row>
-    <row r="105" spans="1:7" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D104" s="4"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="29"/>
+    </row>
+    <row r="105" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>43002</v>
       </c>
@@ -2441,10 +2558,11 @@
         <v>Sunday</v>
       </c>
       <c r="C105" s="4"/>
-      <c r="F105" s="28"/>
-      <c r="G105" s="29"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D105" s="4"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="29"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>43003</v>
       </c>
@@ -2455,10 +2573,11 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
-      <c r="F106" s="27"/>
+      <c r="F106" s="7"/>
       <c r="G106" s="27"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="27"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>43004</v>
       </c>
@@ -2469,10 +2588,11 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
-      <c r="F107" s="27"/>
+      <c r="F107" s="7"/>
       <c r="G107" s="27"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="27"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>43005</v>
       </c>
@@ -2483,10 +2603,11 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
-      <c r="F108" s="27"/>
+      <c r="F108" s="7"/>
       <c r="G108" s="27"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="27"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>43006</v>
       </c>
@@ -2497,10 +2618,11 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
-      <c r="F109" s="27"/>
+      <c r="F109" s="7"/>
       <c r="G109" s="27"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="27"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>43007</v>
       </c>
@@ -2511,10 +2633,11 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
-      <c r="F110" s="27"/>
+      <c r="F110" s="7"/>
       <c r="G110" s="27"/>
-    </row>
-    <row r="111" spans="1:7" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H110" s="27"/>
+    </row>
+    <row r="111" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>43008</v>
       </c>
@@ -2525,6 +2648,7 @@
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B111">
@@ -2539,9 +2663,9 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="3">
-    <mergeCell ref="E3:E12"/>
-    <mergeCell ref="F2:F110"/>
+    <mergeCell ref="F3:F12"/>
     <mergeCell ref="G2:G110"/>
+    <mergeCell ref="H2:H110"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B111">
     <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastMonth">

</xml_diff>

<commit_message>
Updated focus event in DatepickBox. Other minor changes.
</commit_message>
<xml_diff>
--- a/docs/dev-plan-draft.xlsx
+++ b/docs/dev-plan-draft.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">Checkbox design of unsolicited response </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data population in all input boxes - both basic and advanced search </t>
   </si>
   <si>
     <t>Reports page layout</t>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>State ( Green is done, yellow is not required )</t>
+  </si>
+  <si>
+    <t>Data population in all input boxes - availble in an JS object to make searches.</t>
   </si>
 </sst>
 </file>
@@ -386,13 +386,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,12 +466,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -496,6 +490,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -511,10 +508,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -846,25 +846,25 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="38.28515625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="38.42578125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="15.85546875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="38.42578125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -872,22 +872,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>73</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -899,16 +899,16 @@
         <v>Tuesday</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="30"/>
+        <v>77</v>
+      </c>
+      <c r="D2" s="15"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>79</v>
+      <c r="G2" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -924,11 +924,11 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="F3" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -941,11 +941,11 @@
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -958,11 +958,11 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -972,9 +972,9 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -985,9 +985,9 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1001,11 +1001,11 @@
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="31"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1018,11 +1018,11 @@
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="31"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -1035,11 +1035,11 @@
       <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="31"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1052,11 +1052,11 @@
       <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1069,11 +1069,11 @@
       <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1087,8 +1087,8 @@
         <v>6</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
       <c r="I13" s="8"/>
     </row>
     <row r="14" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1101,8 +1101,8 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
       <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1116,11 +1116,11 @@
       <c r="C15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="31"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1133,11 +1133,11 @@
       <c r="C16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -1148,13 +1148,13 @@
         <v>Wednesday</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1170,8 +1170,8 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -1187,8 +1187,8 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1202,8 +1202,8 @@
         <v>10</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1214,8 +1214,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1232,8 +1232,8 @@
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -1249,8 +1249,8 @@
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1266,8 +1266,8 @@
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -1280,11 +1280,11 @@
       <c r="C25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="31"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1297,11 +1297,11 @@
       <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="31"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
     </row>
     <row r="27" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -1311,8 +1311,8 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1323,8 +1323,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="29"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28"/>
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1338,11 +1338,11 @@
       <c r="C29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="31"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1358,8 +1358,8 @@
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -1375,8 +1375,8 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -1392,8 +1392,8 @@
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -1406,11 +1406,11 @@
       <c r="C33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
     </row>
     <row r="34" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -1420,8 +1420,8 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="G34" s="28"/>
-      <c r="H34" s="29"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="28"/>
       <c r="I34" s="8"/>
     </row>
     <row r="35" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1432,8 +1432,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G35" s="28"/>
-      <c r="H35" s="29"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="28"/>
       <c r="I35" s="8"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1447,11 +1447,11 @@
       <c r="C36" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="7"/>
+      <c r="D36" s="15"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
@@ -1464,11 +1464,11 @@
       <c r="C37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -1481,11 +1481,11 @@
       <c r="C38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="31"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -1501,8 +1501,8 @@
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
@@ -1518,8 +1518,8 @@
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
     </row>
     <row r="41" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -1529,8 +1529,8 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="G41" s="28"/>
-      <c r="H41" s="29"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="28"/>
       <c r="I41" s="8"/>
     </row>
     <row r="42" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,8 +1541,8 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="29"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="28"/>
       <c r="I42" s="8"/>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1559,8 +1559,8 @@
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1571,13 +1571,13 @@
         <v>Tuesday</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
     </row>
     <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
@@ -1588,13 +1588,13 @@
         <v>Wednesday</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
@@ -1605,15 +1605,15 @@
         <v>Thursday</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-    </row>
-    <row r="47" spans="1:9" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+    </row>
+    <row r="47" spans="1:9" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>42944</v>
       </c>
@@ -1622,15 +1622,15 @@
         <v>Friday</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
+        <v>31</v>
+      </c>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
     </row>
     <row r="48" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -1642,8 +1642,8 @@
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="29"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="28"/>
       <c r="I48" s="8"/>
     </row>
     <row r="49" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1656,8 +1656,8 @@
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="29"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="28"/>
       <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1669,15 +1669,15 @@
         <v>Monday</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F50" s="7"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
@@ -1688,15 +1688,15 @@
         <v>Tuesday</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-    </row>
-    <row r="52" spans="1:9" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>42949</v>
       </c>
@@ -1705,15 +1705,15 @@
         <v>Wednesday</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
+        <v>32</v>
+      </c>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
     </row>
     <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1724,15 +1724,15 @@
         <v>Thursday</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="31"/>
+        <v>28</v>
+      </c>
+      <c r="D53" s="23"/>
       <c r="E53" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F53" s="7"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1743,13 +1743,13 @@
         <v>Friday</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D54" s="31"/>
+        <v>33</v>
+      </c>
+      <c r="D54" s="23"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -1761,8 +1761,8 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="29"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="28"/>
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
@@ -1774,8 +1774,8 @@
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="29"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="28"/>
     </row>
     <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1786,13 +1786,13 @@
         <v>Monday</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D57" s="31"/>
+        <v>34</v>
+      </c>
+      <c r="D57" s="23"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
@@ -1803,13 +1803,13 @@
         <v>Tuesday</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="31"/>
+        <v>35</v>
+      </c>
+      <c r="D58" s="23"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -1820,13 +1820,13 @@
         <v>Wednesday</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D59" s="31"/>
+        <v>36</v>
+      </c>
+      <c r="D59" s="23"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
@@ -1837,13 +1837,13 @@
         <v>Thursday</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" s="31"/>
+        <v>37</v>
+      </c>
+      <c r="D60" s="23"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
@@ -1854,13 +1854,13 @@
         <v>Friday</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D61" s="31"/>
+        <v>38</v>
+      </c>
+      <c r="D61" s="23"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
     </row>
     <row r="62" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
@@ -1872,8 +1872,8 @@
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="29"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="28"/>
     </row>
     <row r="63" spans="1:9" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
@@ -1885,8 +1885,8 @@
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="29"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="28"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -1897,13 +1897,13 @@
         <v>Monday</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" s="31"/>
+        <v>39</v>
+      </c>
+      <c r="D64" s="23"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
     </row>
     <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
@@ -1914,13 +1914,13 @@
         <v>Tuesday</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" s="31"/>
+        <v>46</v>
+      </c>
+      <c r="D65" s="23"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
@@ -1931,13 +1931,13 @@
         <v>Wednesday</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66" s="31"/>
+        <v>47</v>
+      </c>
+      <c r="D66" s="23"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="26"/>
     </row>
     <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
@@ -1948,15 +1948,15 @@
         <v>Thursday</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="D67" s="23"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
+        <v>48</v>
+      </c>
+      <c r="G67" s="26"/>
+      <c r="H67" s="26"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
@@ -1967,13 +1967,13 @@
         <v>Friday</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="D68" s="23"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="27"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
     </row>
     <row r="69" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -1983,8 +1983,8 @@
         <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
-      <c r="G69" s="28"/>
-      <c r="H69" s="29"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="28"/>
     </row>
     <row r="70" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
@@ -1994,8 +1994,8 @@
         <f t="shared" si="1"/>
         <v>Sunday</v>
       </c>
-      <c r="G70" s="28"/>
-      <c r="H70" s="29"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="28"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
@@ -2006,13 +2006,13 @@
         <v>Monday</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D71" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="D71" s="23"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
-      <c r="G71" s="27"/>
-      <c r="H71" s="27"/>
+      <c r="G71" s="26"/>
+      <c r="H71" s="26"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
@@ -2023,13 +2023,13 @@
         <v>Tuesday</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="D72" s="23"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="26"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
@@ -2040,13 +2040,13 @@
         <v>Wednesday</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D73" s="31"/>
+        <v>45</v>
+      </c>
+      <c r="D73" s="23"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="26"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
@@ -2057,13 +2057,13 @@
         <v>Thursday</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D74" s="31"/>
+        <v>42</v>
+      </c>
+      <c r="D74" s="23"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="27"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
@@ -2074,13 +2074,13 @@
         <v>Friday</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D75" s="31"/>
+        <v>43</v>
+      </c>
+      <c r="D75" s="23"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
+      <c r="G75" s="26"/>
+      <c r="H75" s="26"/>
     </row>
     <row r="76" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
@@ -2092,8 +2092,8 @@
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
-      <c r="G76" s="28"/>
-      <c r="H76" s="29"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="28"/>
     </row>
     <row r="77" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
@@ -2105,8 +2105,8 @@
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="29"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="28"/>
     </row>
     <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
@@ -2117,13 +2117,13 @@
         <v>Monday</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D78" s="31"/>
+        <v>44</v>
+      </c>
+      <c r="D78" s="23"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
-      <c r="G78" s="27"/>
-      <c r="H78" s="27"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="26"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
@@ -2134,13 +2134,13 @@
         <v>Tuesday</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D79" s="31"/>
+        <v>50</v>
+      </c>
+      <c r="D79" s="23"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
-      <c r="G79" s="27"/>
-      <c r="H79" s="27"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="26"/>
     </row>
     <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
@@ -2151,15 +2151,15 @@
         <v>Wednesday</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D80" s="31"/>
+        <v>52</v>
+      </c>
+      <c r="D80" s="23"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
+        <v>51</v>
+      </c>
+      <c r="G80" s="26"/>
+      <c r="H80" s="26"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
@@ -2170,15 +2170,15 @@
         <v>Thursday</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D81" s="31"/>
+        <v>53</v>
+      </c>
+      <c r="D81" s="23"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-    </row>
-    <row r="82" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
+    </row>
+    <row r="82" spans="1:8" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>42979</v>
       </c>
@@ -2187,15 +2187,15 @@
         <v>Friday</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D82" s="31"/>
+        <v>54</v>
+      </c>
+      <c r="D82" s="23"/>
       <c r="E82" s="11"/>
       <c r="F82" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
+        <v>56</v>
+      </c>
+      <c r="G82" s="26"/>
+      <c r="H82" s="26"/>
     </row>
     <row r="83" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
@@ -2207,8 +2207,8 @@
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
-      <c r="G83" s="28"/>
-      <c r="H83" s="29"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="28"/>
     </row>
     <row r="84" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
@@ -2220,10 +2220,10 @@
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
-      <c r="G84" s="28"/>
-      <c r="H84" s="29"/>
-    </row>
-    <row r="85" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G84" s="27"/>
+      <c r="H84" s="28"/>
+    </row>
+    <row r="85" spans="1:8" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>42982</v>
       </c>
@@ -2232,13 +2232,13 @@
         <v>Monday</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D85" s="31"/>
+        <v>55</v>
+      </c>
+      <c r="D85" s="23"/>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
-      <c r="G85" s="27"/>
-      <c r="H85" s="27"/>
+      <c r="G85" s="26"/>
+      <c r="H85" s="26"/>
     </row>
     <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
@@ -2249,15 +2249,15 @@
         <v>Tuesday</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F86" s="7"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
     </row>
     <row r="87" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
@@ -2268,13 +2268,13 @@
         <v>Wednesday</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="27"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="26"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
@@ -2285,13 +2285,13 @@
         <v>Thursday</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="27"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="26"/>
     </row>
     <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
@@ -2302,13 +2302,13 @@
         <v>Friday</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
+      <c r="G89" s="26"/>
+      <c r="H89" s="26"/>
     </row>
     <row r="90" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
@@ -2320,8 +2320,8 @@
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="29"/>
+      <c r="G90" s="27"/>
+      <c r="H90" s="28"/>
     </row>
     <row r="91" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
@@ -2333,8 +2333,8 @@
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
-      <c r="G91" s="28"/>
-      <c r="H91" s="29"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="28"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
@@ -2345,13 +2345,13 @@
         <v>Monday</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
+      <c r="G92" s="26"/>
+      <c r="H92" s="26"/>
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
@@ -2362,13 +2362,13 @@
         <v>Tuesday</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="27"/>
+      <c r="G93" s="26"/>
+      <c r="H93" s="26"/>
     </row>
     <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
@@ -2379,13 +2379,13 @@
         <v>Wednesday</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
-      <c r="G94" s="27"/>
-      <c r="H94" s="27"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="26"/>
     </row>
     <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
@@ -2396,15 +2396,15 @@
         <v>Thursday</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="27"/>
-    </row>
-    <row r="96" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G95" s="26"/>
+      <c r="H95" s="26"/>
+    </row>
+    <row r="96" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>42993</v>
       </c>
@@ -2413,15 +2413,15 @@
         <v>Friday</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G96" s="27"/>
-      <c r="H96" s="27"/>
+        <v>49</v>
+      </c>
+      <c r="G96" s="26"/>
+      <c r="H96" s="26"/>
     </row>
     <row r="97" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
@@ -2433,8 +2433,8 @@
       </c>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="G97" s="28"/>
-      <c r="H97" s="29"/>
+      <c r="G97" s="27"/>
+      <c r="H97" s="28"/>
     </row>
     <row r="98" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
@@ -2446,8 +2446,8 @@
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="G98" s="28"/>
-      <c r="H98" s="29"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="28"/>
     </row>
     <row r="99" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
@@ -2458,51 +2458,51 @@
         <v>Monday</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F99" s="7"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-    </row>
-    <row r="100" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="15">
+      <c r="G99" s="26"/>
+      <c r="H99" s="26"/>
+    </row>
+    <row r="100" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="30">
         <v>42997</v>
       </c>
-      <c r="B100" s="16" t="str">
+      <c r="B100" s="31" t="str">
         <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
-      <c r="C100" s="17" t="s">
+      <c r="C100" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G100" s="27"/>
-      <c r="H100" s="27"/>
-    </row>
-    <row r="101" spans="1:8" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="15">
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
+    </row>
+    <row r="101" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="30">
         <v>42998</v>
       </c>
-      <c r="B101" s="16" t="str">
+      <c r="B101" s="31" t="str">
         <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
-      <c r="C101" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
-      <c r="F101" s="17"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
+      <c r="C101" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
     </row>
     <row r="102" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
@@ -2515,11 +2515,11 @@
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F102" s="7"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
+      <c r="G102" s="26"/>
+      <c r="H102" s="26"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
@@ -2533,8 +2533,8 @@
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
-      <c r="G103" s="27"/>
-      <c r="H103" s="27"/>
+      <c r="G103" s="26"/>
+      <c r="H103" s="26"/>
     </row>
     <row r="104" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
@@ -2546,8 +2546,8 @@
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
-      <c r="G104" s="28"/>
-      <c r="H104" s="29"/>
+      <c r="G104" s="27"/>
+      <c r="H104" s="28"/>
     </row>
     <row r="105" spans="1:8" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
@@ -2559,8 +2559,8 @@
       </c>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="29"/>
+      <c r="G105" s="27"/>
+      <c r="H105" s="28"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
@@ -2574,8 +2574,8 @@
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
-      <c r="G106" s="27"/>
-      <c r="H106" s="27"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="26"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
@@ -2589,8 +2589,8 @@
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
+      <c r="G107" s="26"/>
+      <c r="H107" s="26"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
@@ -2604,8 +2604,8 @@
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="27"/>
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
@@ -2619,8 +2619,8 @@
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
+      <c r="G109" s="26"/>
+      <c r="H109" s="26"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
@@ -2634,8 +2634,8 @@
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
-      <c r="G110" s="27"/>
-      <c r="H110" s="27"/>
+      <c r="G110" s="26"/>
+      <c r="H110" s="26"/>
     </row>
     <row r="111" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">

</xml_diff>

<commit_message>
Added search button loading image.
</commit_message>
<xml_diff>
--- a/docs/dev-plan-draft.xlsx
+++ b/docs/dev-plan-draft.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="13950" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>Data population in all input boxes - availble in an JS object to make searches.</t>
+  </si>
+  <si>
+    <t>Message Box of error design</t>
   </si>
 </sst>
 </file>
@@ -846,8 +849,8 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C87" sqref="C87"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,9 +1230,9 @@
         <v>Monday</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="D22" s="15"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="29"/>

</xml_diff>

<commit_message>
Working on search button status.
</commit_message>
<xml_diff>
--- a/docs/dev-plan-draft.xlsx
+++ b/docs/dev-plan-draft.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="14880" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -849,8 +849,8 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>